<commit_message>
erster versuch mit sql
</commit_message>
<xml_diff>
--- a/Versandbestätigungsvorlage.xlsx
+++ b/Versandbestätigungsvorlage.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr date1904="1" filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D13419-32F8-4357-8FFD-78BAECDC58AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3D55D4-EC53-4E31-9044-C2DDA534102F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="46">
   <si>
     <t>Bestell-ID</t>
   </si>
@@ -60,16 +60,100 @@
     <t>Die Versandnummer für den Versand des Artikels.</t>
   </si>
   <si>
-    <t>PO-076-02524995022710164</t>
+    <t>PO-076-18846061310073237</t>
   </si>
   <si>
     <t>Hünxe</t>
   </si>
   <si>
-    <t>01465054486544</t>
-  </si>
-  <si>
-    <t>DPD (DE)</t>
+    <t>DHL Paket</t>
+  </si>
+  <si>
+    <t>PO-076-07774644721273946</t>
+  </si>
+  <si>
+    <t>PO-076-19057247396470472</t>
+  </si>
+  <si>
+    <t>PO-076-08044892923510289</t>
+  </si>
+  <si>
+    <t>PO-076-03299690250872749</t>
+  </si>
+  <si>
+    <t>PO-076-19026772655990366</t>
+  </si>
+  <si>
+    <t>PO-076-07627727094393062</t>
+  </si>
+  <si>
+    <t>PO-076-18616847544952843</t>
+  </si>
+  <si>
+    <t>PO-076-19040316124790319</t>
+  </si>
+  <si>
+    <t>PO-076-03340413676152984</t>
+  </si>
+  <si>
+    <t>00340434288253297839</t>
+  </si>
+  <si>
+    <t>00340434288253297808</t>
+  </si>
+  <si>
+    <t>00340434288253297860</t>
+  </si>
+  <si>
+    <t>00340434288253297815</t>
+  </si>
+  <si>
+    <t>00340434288253297785</t>
+  </si>
+  <si>
+    <t>00340434288253297846</t>
+  </si>
+  <si>
+    <t>00340434288253297792</t>
+  </si>
+  <si>
+    <t>00340434288253297822</t>
+  </si>
+  <si>
+    <t>00340434288253297853</t>
+  </si>
+  <si>
+    <t>00340434288253298935</t>
+  </si>
+  <si>
+    <t>076-03340455619192984</t>
+  </si>
+  <si>
+    <t>076-07627685151353062</t>
+  </si>
+  <si>
+    <t>076-08044856223350289</t>
+  </si>
+  <si>
+    <t>076-07774592292473946</t>
+  </si>
+  <si>
+    <t>076-19040420982390319</t>
+  </si>
+  <si>
+    <t>076-19057273610870472</t>
+  </si>
+  <si>
+    <t>076-18846053445753237</t>
+  </si>
+  <si>
+    <t>076-18616852787832843</t>
+  </si>
+  <si>
+    <t>076-19026751684470366</t>
+  </si>
+  <si>
+    <t>076-03299737436792749</t>
   </si>
 </sst>
 </file>
@@ -148,11 +232,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -493,16 +577,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="30" style="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" style="1" customWidth="1"/>
+    <col min="2" max="5" width="30" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -521,7 +607,7 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
@@ -529,14 +615,200 @@
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>16</v>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>